<commit_message>
removed test column from example dataset
</commit_message>
<xml_diff>
--- a/data/toy_animal_trial_data_long.xlsx
+++ b/data/toy_animal_trial_data_long.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicola-palmieri/Dropbox/Personal/GitHub/TableAnalyzer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palmi\Dropbox\Personal\GitHub\TableAnalyzer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A03F0ED-5F7D-CE4E-B181-6D3718B23E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8389EB-FAAB-479B-9D10-A67F60B1D1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="620" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="145">
   <si>
     <t>Treatment</t>
   </si>
@@ -455,9 +455,6 @@
   </si>
   <si>
     <t>A057</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -810,15 +807,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M121"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,11 +852,8 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -896,11 +890,8 @@
       <c r="L2">
         <v>39.111469200824551</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -937,11 +928,8 @@
       <c r="L3">
         <v>39.044780546499368</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -978,11 +966,8 @@
       <c r="L4">
         <v>38.71374187929446</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1019,11 +1004,8 @@
       <c r="L5">
         <v>38.647198817834507</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1060,11 +1042,8 @@
       <c r="L6">
         <v>39.03776155046841</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1101,11 +1080,8 @@
       <c r="L7">
         <v>39.179051142377858</v>
       </c>
-      <c r="M7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1142,11 +1118,8 @@
       <c r="L8">
         <v>38.944722524811773</v>
       </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1183,11 +1156,8 @@
       <c r="L9">
         <v>38.993999767708807</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1225,7 +1195,7 @@
         <v>38.502699262313683</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1263,7 +1233,7 @@
         <v>38.606703187641848</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1301,7 +1271,7 @@
         <v>38.253351061298737</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1339,7 +1309,7 @@
         <v>38.694232874812258</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1377,7 +1347,7 @@
         <v>38.658558629987127</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1415,7 +1385,7 @@
         <v>38.653173315323222</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1453,7 +1423,7 @@
         <v>39.044704243174891</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1491,7 +1461,7 @@
         <v>38.697366459409572</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1529,7 +1499,7 @@
         <v>38.367940834004877</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1537,7 @@
         <v>39.084239487922957</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1605,7 +1575,7 @@
         <v>38.922821885959443</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1643,7 +1613,7 @@
         <v>39.334199461079628</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1681,7 +1651,7 @@
         <v>38.808448543345627</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1719,7 +1689,7 @@
         <v>38.52686202788226</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1757,7 +1727,7 @@
         <v>38.964019160008327</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1795,7 +1765,7 @@
         <v>38.841937712252317</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1833,7 +1803,7 @@
         <v>38.784057130524232</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1871,7 +1841,7 @@
         <v>39.202070606490423</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1909,7 +1879,7 @@
         <v>39.23580079330808</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1947,7 +1917,7 @@
         <v>39.088954919583522</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1985,7 +1955,7 @@
         <v>39.35226118031305</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2023,7 +1993,7 @@
         <v>39.261725907349742</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -2061,7 +2031,7 @@
         <v>38.962311914748113</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2099,7 +2069,7 @@
         <v>38.932942803714788</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2137,7 +2107,7 @@
         <v>38.699056029494713</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2175,7 +2145,7 @@
         <v>38.900094209617762</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -2213,7 +2183,7 @@
         <v>39.381617288372098</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2251,7 +2221,7 @@
         <v>38.558703081358082</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2289,7 +2259,7 @@
         <v>38.738212478264558</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2327,7 +2297,7 @@
         <v>38.809955864633743</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2365,7 +2335,7 @@
         <v>38.830225193909342</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2373,7 @@
         <v>38.945016603534967</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2441,7 +2411,7 @@
         <v>38.774342292960533</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2479,7 +2449,7 @@
         <v>38.448087471347712</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2517,7 +2487,7 @@
         <v>38.709419422692562</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2555,7 +2525,7 @@
         <v>38.73143896212661</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2593,7 +2563,7 @@
         <v>38.297852933472953</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2631,7 +2601,7 @@
         <v>38.644888128605537</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2669,7 +2639,7 @@
         <v>38.685424919853197</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -2707,7 +2677,7 @@
         <v>38.31669306659569</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2745,7 +2715,7 @@
         <v>38.833593614911621</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -2783,7 +2753,7 @@
         <v>39.136523627058367</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -2821,7 +2791,7 @@
         <v>38.444444487844549</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2829,7 @@
         <v>38.82319689288056</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2897,7 +2867,7 @@
         <v>39.158947472641337</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2935,7 +2905,7 @@
         <v>38.948883715380099</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -2973,7 +2943,7 @@
         <v>39.00335479555195</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -3011,7 +2981,7 @@
         <v>39.152813210133182</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -3049,7 +3019,7 @@
         <v>38.935409937630723</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>22</v>
       </c>
@@ -3087,7 +3057,7 @@
         <v>38.083437246739337</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -3125,7 +3095,7 @@
         <v>38.693340584178927</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -3163,7 +3133,7 @@
         <v>38.722602704439467</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -3201,7 +3171,7 @@
         <v>38.699636037599447</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -3239,7 +3209,7 @@
         <v>38.689235029809829</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -3277,7 +3247,7 @@
         <v>38.759668653676322</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -3315,7 +3285,7 @@
         <v>38.441405713903862</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3353,7 +3323,7 @@
         <v>38.777321648570663</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -3391,7 +3361,7 @@
         <v>38.829420303580612</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>22</v>
       </c>
@@ -3429,7 +3399,7 @@
         <v>38.843476042187817</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -3467,7 +3437,7 @@
         <v>38.920920725345162</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -3505,7 +3475,7 @@
         <v>38.518753580562041</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -3543,7 +3513,7 @@
         <v>38.677391961256838</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -3581,7 +3551,7 @@
         <v>39.009082876289362</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -3619,7 +3589,7 @@
         <v>38.88621498186707</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -3657,7 +3627,7 @@
         <v>39.073276299387757</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>22</v>
       </c>
@@ -3695,7 +3665,7 @@
         <v>38.454331476581103</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -3733,7 +3703,7 @@
         <v>39.176035980238296</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -3771,7 +3741,7 @@
         <v>38.969759914317137</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -3809,7 +3779,7 @@
         <v>38.68801065014808</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -3847,7 +3817,7 @@
         <v>38.378387965011058</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -3885,7 +3855,7 @@
         <v>38.266379802010668</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -3923,7 +3893,7 @@
         <v>38.310043240791607</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -3961,7 +3931,7 @@
         <v>38.948834672809667</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -3999,7 +3969,7 @@
         <v>39.26960563754583</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -4037,7 +4007,7 @@
         <v>39.309474445137027</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -4075,7 +4045,7 @@
         <v>39.06535999426773</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -4113,7 +4083,7 @@
         <v>38.260007691115447</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -4151,7 +4121,7 @@
         <v>38.367326616676159</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -4189,7 +4159,7 @@
         <v>38.989144195745112</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -4227,7 +4197,7 @@
         <v>38.382380427743414</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -4265,7 +4235,7 @@
         <v>38.73231201418362</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -4303,7 +4273,7 @@
         <v>38.554463607694892</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -4341,7 +4311,7 @@
         <v>38.75190629115356</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -4379,7 +4349,7 @@
         <v>38.766233451801916</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -4417,7 +4387,7 @@
         <v>38.826967584648862</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -4455,7 +4425,7 @@
         <v>39.100208061978897</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>22</v>
       </c>
@@ -4493,7 +4463,7 @@
         <v>38.932645828903958</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -4531,7 +4501,7 @@
         <v>38.984461271494723</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -4569,7 +4539,7 @@
         <v>38.855209406095263</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -4607,7 +4577,7 @@
         <v>38.474363901005653</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>22</v>
       </c>
@@ -4645,7 +4615,7 @@
         <v>38.840990768160047</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -4683,7 +4653,7 @@
         <v>38.806228086227122</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -4721,7 +4691,7 @@
         <v>38.793494572578979</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>22</v>
       </c>
@@ -4759,7 +4729,7 @@
         <v>38.143792747969492</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -4797,7 +4767,7 @@
         <v>38.79617184616621</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>22</v>
       </c>
@@ -4835,7 +4805,7 @@
         <v>38.325141464842837</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>22</v>
       </c>
@@ -4873,7 +4843,7 @@
         <v>38.635071112485512</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -4911,7 +4881,7 @@
         <v>39.186285386557948</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -4949,7 +4919,7 @@
         <v>38.831860016353801</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -4987,7 +4957,7 @@
         <v>39.842239791353457</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -5025,7 +4995,7 @@
         <v>38.593433474879447</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>22</v>
       </c>
@@ -5063,7 +5033,7 @@
         <v>38.648479031514462</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>22</v>
       </c>
@@ -5101,7 +5071,7 @@
         <v>38.049373510286358</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -5139,7 +5109,7 @@
         <v>38.757925394525813</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>12</v>
       </c>
@@ -5177,7 +5147,7 @@
         <v>38.635920240062802</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -5215,7 +5185,7 @@
         <v>39.161027278644823</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>22</v>
       </c>
@@ -5253,7 +5223,7 @@
         <v>38.550763587676421</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -5291,7 +5261,7 @@
         <v>38.436201857834767</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -5329,7 +5299,7 @@
         <v>38.958104896189418</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -5367,7 +5337,7 @@
         <v>38.934945105466262</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>12</v>
       </c>
@@ -5405,7 +5375,7 @@
         <v>38.69737986952569</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>18</v>
       </c>

</xml_diff>